<commit_message>
Update: Threat Alert Report - 2026-01-18 01:00
</commit_message>
<xml_diff>
--- a/excel_routes/route_AHB_ATZ_threats.xlsx
+++ b/excel_routes/route_AHB_ATZ_threats.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,7 +528,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>06-FEB-26</t>
+          <t>13-FEB-26</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -565,51 +565,6 @@
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>SAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>13-FEB-26</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>SM-446</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Air Arabia Egypt E5-512</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>594</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>895</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>-301</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
         <is>
           <t>SAR</t>
         </is>

</xml_diff>

<commit_message>
Update: Threat Alert Report - 2026-01-18 10:31
</commit_message>
<xml_diff>
--- a/excel_routes/route_AHB_ATZ_threats.xlsx
+++ b/excel_routes/route_AHB_ATZ_threats.xlsx
@@ -1,55 +1,121 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODERED\LAB\Artifacts\outputs\run_generated_170126_at_23.33_RETRY\reports\excel_routes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F0D359-B824-4447-A5CD-17048BF663A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="THREAT_ALERT" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="THREAT_ALERT" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Air Cairo Flight</t>
+  </si>
+  <si>
+    <t>Market Threat Airline</t>
+  </si>
+  <si>
+    <t>OAL Fare Threat</t>
+  </si>
+  <si>
+    <t>Our Fare</t>
+  </si>
+  <si>
+    <t>Fare Dif</t>
+  </si>
+  <si>
+    <t>OAL Baggage</t>
+  </si>
+  <si>
+    <t>Our Baggage</t>
+  </si>
+  <si>
+    <t>Bag Allowance Dif</t>
+  </si>
+  <si>
+    <t>IMPACT</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>13-FEB-26</t>
+  </si>
+  <si>
+    <t>SM-446</t>
+  </si>
+  <si>
+    <t>Air Arabia Egypt E5-512</t>
+  </si>
+  <si>
+    <t>LOW THREAT</t>
+  </si>
+  <si>
+    <t>SAR</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="003498DB"/>
-        <bgColor rgb="003498DB"/>
+        <fgColor rgb="FF3498DB"/>
+        <bgColor rgb="FF3498DB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D4EDDA"/>
-        <bgColor rgb="00D4EDDA"/>
+        <fgColor rgb="FFD4EDDA"/>
+        <bgColor rgb="FFD4EDDA"/>
       </patternFill>
     </fill>
   </fills>
@@ -62,99 +128,49 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -442,132 +458,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="25" customWidth="1" min="3" max="3"/>
-    <col width="17" customWidth="1" min="4" max="4"/>
-    <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
-    <col width="13" customWidth="1" min="8" max="8"/>
-    <col width="19" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="10" customWidth="1" min="11" max="11"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="153.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Air Cairo Flight</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Market Threat Airline</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>OAL Fare Threat</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Our Fare</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Fare Dif</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>OAL Baggage</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Our Baggage</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Bag Allowance Dif</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>IMPACT</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Currency</t>
-        </is>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>13-FEB-26</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>SM-446</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>Air Arabia Egypt E5-512</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2">
         <v>594</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="2">
         <v>895</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <v>-301</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="2">
         <v>30</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="2">
         <v>30</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>SAR</t>
-        </is>
+      <c r="J2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: Threat Alert Report - 2026-01-25 09:07
</commit_message>
<xml_diff>
--- a/excel_routes/route_AHB_ATZ_threats.xlsx
+++ b/excel_routes/route_AHB_ATZ_threats.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,7 +528,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>13-MAR-26</t>
+          <t>30-JAN-26</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>1181</v>
+        <v>612</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>1501</v>
+        <v>895</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>-320</v>
+        <v>-283</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>30</v>
@@ -565,6 +565,96 @@
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>SAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>20-FEB-26</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>SM-446</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Air Arabia Egypt E5-512</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>513</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>883</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>-370</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>LOW THREAT</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>SAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>27-FEB-26</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>SM-446</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Air Arabia Egypt E5-512</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>513</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>786</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>-273</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>LOW THREAT</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
         <is>
           <t>SAR</t>
         </is>

</xml_diff>

<commit_message>
Update: Threat Alert Report - 2026-01-30 06:29
</commit_message>
<xml_diff>
--- a/excel_routes/route_AHB_ATZ_threats.xlsx
+++ b/excel_routes/route_AHB_ATZ_threats.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,7 +528,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>30-JAN-26</t>
+          <t>13-FEB-26</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>612</v>
+        <v>687</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>895</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>-283</v>
+        <v>-208</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>30</v>
@@ -618,7 +618,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>27-FEB-26</t>
+          <t>13-MAR-26</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -632,13 +632,13 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>513</v>
+        <v>1237</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>786</v>
+        <v>1501</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>-273</v>
+        <v>-264</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>30</v>
@@ -655,6 +655,51 @@
         </is>
       </c>
       <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>SAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>27-MAR-26</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>SM-446</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Air Arabia Egypt E5-512</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>513</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>786</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>-273</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>LOW THREAT</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
         <is>
           <t>SAR</t>
         </is>

</xml_diff>

<commit_message>
Update: Threat Alert Report - 2026-02-04 14:18
</commit_message>
<xml_diff>
--- a/excel_routes/route_AHB_ATZ_threats.xlsx
+++ b/excel_routes/route_AHB_ATZ_threats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODERED\LAB\Artifacts\outputs\run_generated_030226_at_07.14\reports\excel_routes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODERED\LAB\Artifacts\outputs\run_generated_300126_at_05.16\reports\excel_routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A9180C-393D-4265-A751-AF03AD4607FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2162078D-C387-4855-866A-2514F0789FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>06-FEB-26</t>
+    <t>13-FEB-26</t>
   </si>
   <si>
     <t>SM-446</t>
@@ -75,13 +75,13 @@
     <t>SAR</t>
   </si>
   <si>
-    <t>13-FEB-26</t>
-  </si>
-  <si>
     <t>20-FEB-26</t>
   </si>
   <si>
-    <t>27-FEB-26</t>
+    <t>13-MAR-26</t>
+  </si>
+  <si>
+    <t>27-MAR-26</t>
   </si>
 </sst>
 </file>
@@ -533,13 +533,13 @@
         <v>13</v>
       </c>
       <c r="D2" s="2">
-        <v>837</v>
+        <v>687</v>
       </c>
       <c r="E2" s="2">
-        <v>1159</v>
+        <v>895</v>
       </c>
       <c r="F2" s="2">
-        <v>-322</v>
+        <v>-208</v>
       </c>
       <c r="G2" s="2">
         <v>30</v>
@@ -568,13 +568,13 @@
         <v>13</v>
       </c>
       <c r="D3" s="2">
-        <v>725</v>
+        <v>513</v>
       </c>
       <c r="E3" s="2">
-        <v>1013</v>
+        <v>883</v>
       </c>
       <c r="F3" s="2">
-        <v>-288</v>
+        <v>-370</v>
       </c>
       <c r="G3" s="2">
         <v>30</v>
@@ -603,13 +603,13 @@
         <v>13</v>
       </c>
       <c r="D4" s="2">
-        <v>513</v>
+        <v>1237</v>
       </c>
       <c r="E4" s="2">
-        <v>786</v>
+        <v>1501</v>
       </c>
       <c r="F4" s="2">
-        <v>-273</v>
+        <v>-264</v>
       </c>
       <c r="G4" s="2">
         <v>30</v>
@@ -638,13 +638,13 @@
         <v>13</v>
       </c>
       <c r="D5" s="2">
-        <v>564</v>
+        <v>513</v>
       </c>
       <c r="E5" s="2">
-        <v>883</v>
+        <v>786</v>
       </c>
       <c r="F5" s="2">
-        <v>-319</v>
+        <v>-273</v>
       </c>
       <c r="G5" s="2">
         <v>30</v>

</xml_diff>